<commit_message>
next stage of analysis
</commit_message>
<xml_diff>
--- a/xls/coded_subject_terms.xlsx
+++ b/xls/coded_subject_terms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfoasberg\Desktop\ProjectTRIKE\American_Literature\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nfoasberg\Desktop\ProjectTRIKE\Son_of_Am_Lit\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1124,7 +1124,7 @@
   <dimension ref="A1:C322"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E251" sqref="E251"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>